<commit_message>
update ottchet po ymershim
</commit_message>
<xml_diff>
--- a/Мониторинг_деятельности_лабораторий_01.05.2023.xlsx
+++ b/Мониторинг_деятельности_лабораторий_01.05.2023.xlsx
@@ -811,29 +811,29 @@
       </c>
       <c r="B5" s="9" t="inlineStr">
         <is>
-          <t>СПБ ГБУЗ "Введенская больница"</t>
+          <t>ГБУ СПб НИИ СП им. И.И. Джанелидзе</t>
         </is>
       </c>
       <c r="C5" s="4" t="n">
-        <v>22073</v>
+        <v>29497</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>25720</v>
+        <v>221555</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="F5" s="4" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="G5" s="4" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H5" s="4" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="I5" s="4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" ht="37.9" customHeight="1">
@@ -842,29 +842,29 @@
       </c>
       <c r="B6" s="9" t="inlineStr">
         <is>
-          <t>СПБ ГБУЗ "ДГМКЦ ВМТ им. К.А. Раухфуса"</t>
+          <t>СПБ ГБУЗ "Введенская больница"</t>
         </is>
       </c>
       <c r="C6" s="4" t="n">
-        <v>20495</v>
+        <v>22073</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>118307</v>
+        <v>25720</v>
       </c>
       <c r="E6" s="4" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F6" s="4" t="n">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="G6" s="4" t="n">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="H6" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I6" s="4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" ht="37.9" customHeight="1">
@@ -873,29 +873,29 @@
       </c>
       <c r="B7" s="9" t="inlineStr">
         <is>
-          <t>СПБ ГБУЗ "Детский городской многопрофильный клинический специализированный центр высоких медицинских технологий"</t>
+          <t>СПБ ГБУЗ "ДГМКЦ ВМТ им. К.А. Раухфуса"</t>
         </is>
       </c>
       <c r="C7" s="4" t="n">
-        <v>77651</v>
+        <v>20495</v>
       </c>
       <c r="D7" s="4" t="n">
-        <v>102528</v>
+        <v>118307</v>
       </c>
       <c r="E7" s="4" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F7" s="4" t="n">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G7" s="4" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H7" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I7" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" ht="37.9" customHeight="1">
@@ -904,29 +904,29 @@
       </c>
       <c r="B8" s="9" t="inlineStr">
         <is>
-          <t>СПБ ГБУЗ "КВД Невского района"</t>
+          <t>СПБ ГБУЗ "Детский городской многопрофильный клинический специализированный центр высоких медицинских технологий"</t>
         </is>
       </c>
       <c r="C8" s="4" t="n">
-        <v>8283</v>
+        <v>77651</v>
       </c>
       <c r="D8" s="4" t="n">
-        <v>14747</v>
+        <v>102528</v>
       </c>
       <c r="E8" s="4" t="n">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F8" s="4" t="n">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="G8" s="4" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="H8" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I8" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" ht="37.9" customHeight="1">
@@ -935,29 +935,29 @@
       </c>
       <c r="B9" s="9" t="inlineStr">
         <is>
-          <t>СПБ ГБУЗ "КВД №1"</t>
+          <t>СПБ ГБУЗ "КВД Невского района"</t>
         </is>
       </c>
       <c r="C9" s="4" t="n">
-        <v>40031</v>
+        <v>8283</v>
       </c>
       <c r="D9" s="4" t="n">
-        <v>98912</v>
+        <v>14747</v>
       </c>
       <c r="E9" s="4" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="F9" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H9" s="4" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I9" s="4" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" ht="37.9" customHeight="1">
@@ -966,29 +966,29 @@
       </c>
       <c r="B10" s="9" t="inlineStr">
         <is>
-          <t>СПБ ГБУЗ "КВД №5"</t>
+          <t>СПБ ГБУЗ "КВД №1"</t>
         </is>
       </c>
       <c r="C10" s="4" t="n">
-        <v>5559</v>
+        <v>40031</v>
       </c>
       <c r="D10" s="4" t="n">
-        <v>2006</v>
+        <v>98912</v>
       </c>
       <c r="E10" s="4" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F10" s="4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G10" s="4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H10" s="4" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I10" s="4" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" ht="37.9" customHeight="1">
@@ -997,20 +997,20 @@
       </c>
       <c r="B11" s="9" t="inlineStr">
         <is>
-          <t>СПБ ГБУЗ "КВД №6"</t>
+          <t>СПБ ГБУЗ "КВД №5"</t>
         </is>
       </c>
       <c r="C11" s="4" t="n">
-        <v>11117</v>
+        <v>5559</v>
       </c>
       <c r="D11" s="4" t="n">
-        <v>25367</v>
+        <v>2006</v>
       </c>
       <c r="E11" s="4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F11" s="4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G11" s="4" t="n">
         <v>1</v>
@@ -1019,7 +1019,7 @@
         <v>2</v>
       </c>
       <c r="I11" s="4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" ht="37.9" customHeight="1">
@@ -1028,26 +1028,26 @@
       </c>
       <c r="B12" s="9" t="inlineStr">
         <is>
-          <t>СПБ ГБУЗ КВД №2</t>
+          <t>СПБ ГБУЗ "КВД №6"</t>
         </is>
       </c>
       <c r="C12" s="4" t="n">
-        <v>26219</v>
+        <v>11117</v>
       </c>
       <c r="D12" s="4" t="n">
-        <v>57275</v>
+        <v>25367</v>
       </c>
       <c r="E12" s="4" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F12" s="4" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G12" s="4" t="n">
         <v>1</v>
       </c>
       <c r="H12" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I12" s="4" t="n">
         <v>2</v>
@@ -1059,23 +1059,23 @@
       </c>
       <c r="B13" s="9" t="inlineStr">
         <is>
-          <t>СПБ ГБУЗ КВД №3</t>
+          <t>СПБ ГБУЗ КВД №11</t>
         </is>
       </c>
       <c r="C13" s="4" t="n">
-        <v>23884</v>
+        <v>44989</v>
       </c>
       <c r="D13" s="4" t="n">
-        <v>41041</v>
+        <v>109021</v>
       </c>
       <c r="E13" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="F13" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="F13" s="4" t="n">
+      <c r="G13" s="4" t="n">
         <v>1</v>
-      </c>
-      <c r="G13" s="4" t="n">
-        <v>0</v>
       </c>
       <c r="H13" s="4" t="n">
         <v>3</v>
@@ -1090,29 +1090,29 @@
       </c>
       <c r="B14" s="9" t="inlineStr">
         <is>
-          <t>СПБ ГБУЗ КВД №4</t>
+          <t>СПБ ГБУЗ КВД №2</t>
         </is>
       </c>
       <c r="C14" s="4" t="n">
-        <v>7899</v>
+        <v>26219</v>
       </c>
       <c r="D14" s="4" t="n">
-        <v>10195</v>
+        <v>57275</v>
       </c>
       <c r="E14" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="F14" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="G14" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="I14" s="4" t="n">
         <v>2</v>
-      </c>
-      <c r="F14" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="I14" s="4" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="15" ht="37.9" customHeight="1">
@@ -1121,14 +1121,14 @@
       </c>
       <c r="B15" s="9" t="inlineStr">
         <is>
-          <t>СПБ ГБУЗ КВД №7</t>
+          <t>СПБ ГБУЗ КВД №3</t>
         </is>
       </c>
       <c r="C15" s="4" t="n">
-        <v>16076</v>
+        <v>23884</v>
       </c>
       <c r="D15" s="4" t="n">
-        <v>25112</v>
+        <v>41041</v>
       </c>
       <c r="E15" s="4" t="n">
         <v>4</v>
@@ -1137,13 +1137,13 @@
         <v>1</v>
       </c>
       <c r="G15" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="4" t="n">
         <v>3</v>
       </c>
       <c r="I15" s="4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" ht="37.9" customHeight="1">
@@ -1152,26 +1152,26 @@
       </c>
       <c r="B16" s="9" t="inlineStr">
         <is>
-          <t>СПБ ГБУЗ КДЦД</t>
+          <t>СПБ ГБУЗ КВД №4</t>
         </is>
       </c>
       <c r="C16" s="4" t="n">
-        <v>130565</v>
+        <v>7899</v>
       </c>
       <c r="D16" s="4" t="n">
-        <v>3331994</v>
+        <v>10195</v>
       </c>
       <c r="E16" s="4" t="n">
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="F16" s="4" t="n">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="G16" s="4" t="n">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="H16" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I16" s="4" t="n">
         <v>0</v>
@@ -1183,29 +1183,29 @@
       </c>
       <c r="B17" s="9" t="inlineStr">
         <is>
-          <t>СПб ГАУЗ "Городская поликлиника №83"</t>
+          <t>СПБ ГБУЗ КВД №7</t>
         </is>
       </c>
       <c r="C17" s="4" t="n">
-        <v>3831</v>
+        <v>16076</v>
       </c>
       <c r="D17" s="4" t="n">
-        <v>22515</v>
+        <v>25112</v>
       </c>
       <c r="E17" s="4" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="F17" s="4" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="G17" s="4" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="H17" s="4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I17" s="4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" ht="37.9" customHeight="1">
@@ -1214,29 +1214,29 @@
       </c>
       <c r="B18" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Александровская больница"</t>
+          <t>СПБ ГБУЗ КДЦД</t>
         </is>
       </c>
       <c r="C18" s="4" t="n">
-        <v>150653</v>
+        <v>130565</v>
       </c>
       <c r="D18" s="4" t="n">
-        <v>680122</v>
+        <v>3331994</v>
       </c>
       <c r="E18" s="4" t="n">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="F18" s="4" t="n">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="G18" s="4" t="n">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="H18" s="4" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I18" s="4" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" ht="37.9" customHeight="1">
@@ -1245,29 +1245,29 @@
       </c>
       <c r="B19" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская Мариинская больница"</t>
+          <t>СПб ГАУЗ "Городская поликлиника №83"</t>
         </is>
       </c>
       <c r="C19" s="4" t="n">
-        <v>99534</v>
+        <v>3831</v>
       </c>
       <c r="D19" s="4" t="n">
-        <v>570865</v>
+        <v>22515</v>
       </c>
       <c r="E19" s="4" t="n">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="F19" s="4" t="n">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="G19" s="4" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="H19" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" ht="37.9" customHeight="1">
@@ -1276,29 +1276,29 @@
       </c>
       <c r="B20" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская Покровская больница"</t>
+          <t>СПб ГБУЗ "Александровская больница"</t>
         </is>
       </c>
       <c r="C20" s="4" t="n">
-        <v>87291</v>
+        <v>150653</v>
       </c>
       <c r="D20" s="4" t="n">
-        <v>256514</v>
+        <v>680122</v>
       </c>
       <c r="E20" s="4" t="n">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="F20" s="4" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G20" s="4" t="n">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="H20" s="4" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="I20" s="4" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" ht="37.9" customHeight="1">
@@ -1307,29 +1307,29 @@
       </c>
       <c r="B21" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская больница Святого Великомученика Георгия"</t>
+          <t>СПб ГБУЗ "Городская Мариинская больница"</t>
         </is>
       </c>
       <c r="C21" s="4" t="n">
-        <v>109257</v>
+        <v>99534</v>
       </c>
       <c r="D21" s="4" t="n">
-        <v>817839</v>
+        <v>570865</v>
       </c>
       <c r="E21" s="4" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F21" s="4" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G21" s="4" t="n">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H21" s="4" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I21" s="4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" ht="37.9" customHeight="1">
@@ -1338,29 +1338,29 @@
       </c>
       <c r="B22" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская больница Святого Праведного Иоанна Кронштадтского"</t>
+          <t>СПб ГБУЗ "Городская Покровская больница"</t>
         </is>
       </c>
       <c r="C22" s="4" t="n">
-        <v>6256</v>
+        <v>87291</v>
       </c>
       <c r="D22" s="4" t="n">
-        <v>24144</v>
+        <v>256514</v>
       </c>
       <c r="E22" s="4" t="n">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="F22" s="4" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="G22" s="4" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H22" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I22" s="4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" ht="37.9" customHeight="1">
@@ -1369,29 +1369,29 @@
       </c>
       <c r="B23" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская больница Святой преподобномученицы Елизаветы"</t>
+          <t>СПб ГБУЗ "Городская больница Святого Великомученика Георгия"</t>
         </is>
       </c>
       <c r="C23" s="4" t="n">
-        <v>121175</v>
+        <v>109257</v>
       </c>
       <c r="D23" s="4" t="n">
-        <v>572677</v>
+        <v>817839</v>
       </c>
       <c r="E23" s="4" t="n">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="F23" s="4" t="n">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G23" s="4" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="H23" s="4" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I23" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" ht="37.9" customHeight="1">
@@ -1400,29 +1400,29 @@
       </c>
       <c r="B24" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская больница №14"</t>
+          <t>СПб ГБУЗ "Городская больница Святого Праведного Иоанна Кронштадтского"</t>
         </is>
       </c>
       <c r="C24" s="4" t="n">
-        <v>10541</v>
+        <v>6256</v>
       </c>
       <c r="D24" s="4" t="n">
-        <v>43867</v>
+        <v>24144</v>
       </c>
       <c r="E24" s="4" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F24" s="4" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G24" s="4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H24" s="4" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I24" s="4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" ht="37.9" customHeight="1">
@@ -1431,26 +1431,26 @@
       </c>
       <c r="B25" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская больница №15"</t>
+          <t>СПб ГБУЗ "Городская больница Святой преподобномученицы Елизаветы"</t>
         </is>
       </c>
       <c r="C25" s="4" t="n">
-        <v>38708</v>
+        <v>121175</v>
       </c>
       <c r="D25" s="4" t="n">
-        <v>119832</v>
+        <v>572677</v>
       </c>
       <c r="E25" s="4" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F25" s="4" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G25" s="4" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H25" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I25" s="4" t="n">
         <v>2</v>
@@ -1462,29 +1462,29 @@
       </c>
       <c r="B26" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская больница №20"</t>
+          <t>СПб ГБУЗ "Городская больница №14"</t>
         </is>
       </c>
       <c r="C26" s="4" t="n">
-        <v>8259</v>
+        <v>10541</v>
       </c>
       <c r="D26" s="4" t="n">
-        <v>24780</v>
+        <v>43867</v>
       </c>
       <c r="E26" s="4" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F26" s="4" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G26" s="4" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H26" s="4" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I26" s="4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" ht="37.9" customHeight="1">
@@ -1493,29 +1493,29 @@
       </c>
       <c r="B27" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская больница №26"</t>
+          <t>СПб ГБУЗ "Городская больница №15"</t>
         </is>
       </c>
       <c r="C27" s="4" t="n">
-        <v>192261</v>
+        <v>38708</v>
       </c>
       <c r="D27" s="4" t="n">
-        <v>619095</v>
+        <v>119832</v>
       </c>
       <c r="E27" s="4" t="n">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F27" s="4" t="n">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="G27" s="4" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H27" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I27" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" ht="37.9" customHeight="1">
@@ -1524,29 +1524,29 @@
       </c>
       <c r="B28" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская больница №28 "Максимилиановская"</t>
+          <t>СПб ГБУЗ "Городская больница №20"</t>
         </is>
       </c>
       <c r="C28" s="4" t="n">
-        <v>2379</v>
+        <v>8259</v>
       </c>
       <c r="D28" s="4" t="n">
-        <v>14156</v>
+        <v>24780</v>
       </c>
       <c r="E28" s="4" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F28" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="G28" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="H28" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G28" s="4" t="n">
+      <c r="I28" s="4" t="n">
         <v>3</v>
-      </c>
-      <c r="H28" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="I28" s="4" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="29" ht="37.9" customHeight="1">
@@ -1555,26 +1555,26 @@
       </c>
       <c r="B29" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская больница №33"</t>
+          <t>СПб ГБУЗ "Городская больница №26"</t>
         </is>
       </c>
       <c r="C29" s="4" t="n">
-        <v>206501</v>
+        <v>192261</v>
       </c>
       <c r="D29" s="4" t="n">
-        <v>945933</v>
+        <v>619095</v>
       </c>
       <c r="E29" s="4" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F29" s="4" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G29" s="4" t="n">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H29" s="4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I29" s="4" t="n">
         <v>1</v>
@@ -1586,29 +1586,29 @@
       </c>
       <c r="B30" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская больница №40"</t>
+          <t>СПб ГБУЗ "Городская больница №28 "Максимилиановская"</t>
         </is>
       </c>
       <c r="C30" s="4" t="n">
-        <v>137448</v>
+        <v>2379</v>
       </c>
       <c r="D30" s="4" t="n">
-        <v>602111</v>
+        <v>14156</v>
       </c>
       <c r="E30" s="4" t="n">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="F30" s="4" t="n">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="G30" s="4" t="n">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="H30" s="4" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I30" s="4" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" ht="37.9" customHeight="1">
@@ -1617,29 +1617,29 @@
       </c>
       <c r="B31" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская больница №9"</t>
+          <t>СПб ГБУЗ "Городская больница №33"</t>
         </is>
       </c>
       <c r="C31" s="4" t="n">
-        <v>6131</v>
+        <v>206501</v>
       </c>
       <c r="D31" s="4" t="n">
-        <v>74950</v>
+        <v>945933</v>
       </c>
       <c r="E31" s="4" t="n">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F31" s="4" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="G31" s="4" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="H31" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I31" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" ht="37.9" customHeight="1">
@@ -1648,29 +1648,29 @@
       </c>
       <c r="B32" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская клиническая больница №31"</t>
+          <t>СПб ГБУЗ "Городская больница №40"</t>
         </is>
       </c>
       <c r="C32" s="4" t="n">
-        <v>14446</v>
+        <v>137448</v>
       </c>
       <c r="D32" s="4" t="n">
-        <v>150542</v>
+        <v>602111</v>
       </c>
       <c r="E32" s="4" t="n">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="F32" s="4" t="n">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="G32" s="4" t="n">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="H32" s="4" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I32" s="4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" ht="37.9" customHeight="1">
@@ -1679,29 +1679,29 @@
       </c>
       <c r="B33" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская многопрофильная больница №2"</t>
+          <t>СПб ГБУЗ "Городская больница №9"</t>
         </is>
       </c>
       <c r="C33" s="4" t="n">
-        <v>84559</v>
+        <v>6131</v>
       </c>
       <c r="D33" s="4" t="n">
-        <v>135452</v>
+        <v>74950</v>
       </c>
       <c r="E33" s="4" t="n">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="F33" s="4" t="n">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="G33" s="4" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="H33" s="4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I33" s="4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" ht="37.9" customHeight="1">
@@ -1710,29 +1710,29 @@
       </c>
       <c r="B34" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская наркологическая больница"</t>
+          <t>СПб ГБУЗ "Городская клиническая больница №31"</t>
         </is>
       </c>
       <c r="C34" s="4" t="n">
-        <v>6443</v>
+        <v>14446</v>
       </c>
       <c r="D34" s="4" t="n">
-        <v>17901</v>
+        <v>150542</v>
       </c>
       <c r="E34" s="4" t="n">
         <v>20</v>
       </c>
       <c r="F34" s="4" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G34" s="4" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H34" s="4" t="n">
         <v>7</v>
       </c>
       <c r="I34" s="4" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" ht="37.9" customHeight="1">
@@ -1741,26 +1741,26 @@
       </c>
       <c r="B35" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская поликлиника №106"</t>
+          <t>СПб ГБУЗ "Городская многопрофильная больница №2"</t>
         </is>
       </c>
       <c r="C35" s="4" t="n">
-        <v>181542</v>
+        <v>84559</v>
       </c>
       <c r="D35" s="4" t="n">
-        <v>880751</v>
+        <v>135452</v>
       </c>
       <c r="E35" s="4" t="n">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F35" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="G35" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="G35" s="4" t="n">
-        <v>19</v>
-      </c>
       <c r="H35" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I35" s="4" t="n">
         <v>2</v>
@@ -1772,29 +1772,29 @@
       </c>
       <c r="B36" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская поликлиника №107"</t>
+          <t>СПб ГБУЗ "Городская наркологическая больница"</t>
         </is>
       </c>
       <c r="C36" s="4" t="n">
-        <v>162979</v>
+        <v>6443</v>
       </c>
       <c r="D36" s="4" t="n">
-        <v>2775709</v>
+        <v>17901</v>
       </c>
       <c r="E36" s="4" t="n">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="F36" s="4" t="n">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="G36" s="4" t="n">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="H36" s="4" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I36" s="4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" ht="37.9" customHeight="1">
@@ -1803,29 +1803,29 @@
       </c>
       <c r="B37" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская поликлиника №112"</t>
+          <t>СПб ГБУЗ "Городская поликлиника №100 Невского района Санкт-Петербурга"</t>
         </is>
       </c>
       <c r="C37" s="4" t="n">
-        <v>5512</v>
+        <v/>
       </c>
       <c r="D37" s="4" t="n">
-        <v>2997</v>
+        <v/>
       </c>
       <c r="E37" s="4" t="n">
-        <v>3</v>
+        <v/>
       </c>
       <c r="F37" s="4" t="n">
-        <v>3</v>
+        <v/>
       </c>
       <c r="G37" s="4" t="n">
-        <v>1</v>
+        <v/>
       </c>
       <c r="H37" s="4" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="I37" s="4" t="n">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="38" ht="37.9" customHeight="1">
@@ -1834,29 +1834,29 @@
       </c>
       <c r="B38" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская поликлиника №118"</t>
+          <t>СПб ГБУЗ "Городская поликлиника №106"</t>
         </is>
       </c>
       <c r="C38" s="4" t="n">
-        <v>5869</v>
+        <v>181542</v>
       </c>
       <c r="D38" s="4" t="n">
-        <v>6862</v>
+        <v>880751</v>
       </c>
       <c r="E38" s="4" t="n">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="F38" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="G38" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="H38" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G38" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H38" s="4" t="n">
-        <v>1</v>
-      </c>
       <c r="I38" s="4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" ht="37.9" customHeight="1">
@@ -1865,26 +1865,26 @@
       </c>
       <c r="B39" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская поликлиника №22"</t>
+          <t>СПб ГБУЗ "Городская поликлиника №107"</t>
         </is>
       </c>
       <c r="C39" s="4" t="n">
-        <v>5799</v>
+        <v>162979</v>
       </c>
       <c r="D39" s="4" t="n">
-        <v>44076</v>
+        <v>2775709</v>
       </c>
       <c r="E39" s="4" t="n">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="F39" s="4" t="n">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="G39" s="4" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="H39" s="4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I39" s="4" t="n">
         <v>0</v>
@@ -1896,26 +1896,26 @@
       </c>
       <c r="B40" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская поликлиника №23"</t>
+          <t>СПб ГБУЗ "Городская поликлиника №112"</t>
         </is>
       </c>
       <c r="C40" s="4" t="n">
-        <v>0</v>
+        <v>5512</v>
       </c>
       <c r="D40" s="4" t="n">
-        <v>0</v>
+        <v>2997</v>
       </c>
       <c r="E40" s="4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F40" s="4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G40" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40" s="4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I40" s="4" t="n">
         <v>0</v>
@@ -1927,26 +1927,26 @@
       </c>
       <c r="B41" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская поликлиника №24"</t>
+          <t>СПб ГБУЗ "Городская поликлиника №118"</t>
         </is>
       </c>
       <c r="C41" s="4" t="n">
-        <v>8004</v>
+        <v>5869</v>
       </c>
       <c r="D41" s="4" t="n">
-        <v>28150</v>
+        <v>6862</v>
       </c>
       <c r="E41" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="F41" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="F41" s="4" t="n">
-        <v>0</v>
-      </c>
       <c r="G41" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H41" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I41" s="4" t="n">
         <v>0</v>
@@ -1958,29 +1958,29 @@
       </c>
       <c r="B42" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская поликлиника №34"</t>
+          <t>СПб ГБУЗ "Городская поликлиника №22"</t>
         </is>
       </c>
       <c r="C42" s="4" t="n">
-        <v>417059</v>
+        <v>5799</v>
       </c>
       <c r="D42" s="4" t="n">
-        <v>1615516</v>
+        <v>44076</v>
       </c>
       <c r="E42" s="4" t="n">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="F42" s="4" t="n">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="G42" s="4" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="H42" s="4" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I42" s="4" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" ht="37.9" customHeight="1">
@@ -1989,26 +1989,26 @@
       </c>
       <c r="B43" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская поликлиника №37"</t>
+          <t>СПб ГБУЗ "Городская поликлиника №23"</t>
         </is>
       </c>
       <c r="C43" s="4" t="n">
-        <v>174</v>
+        <v>0</v>
       </c>
       <c r="D43" s="4" t="n">
-        <v>1912</v>
+        <v>0</v>
       </c>
       <c r="E43" s="4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F43" s="4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G43" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H43" s="4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I43" s="4" t="n">
         <v>0</v>
@@ -2020,29 +2020,29 @@
       </c>
       <c r="B44" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская поликлиника №38"</t>
+          <t>СПб ГБУЗ "Городская поликлиника №24"</t>
         </is>
       </c>
       <c r="C44" s="4" t="n">
-        <v>2016</v>
+        <v>8004</v>
       </c>
       <c r="D44" s="4" t="n">
-        <v>2679</v>
+        <v>28150</v>
       </c>
       <c r="E44" s="4" t="n">
         <v>4</v>
       </c>
       <c r="F44" s="4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G44" s="4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H44" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I44" s="4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" ht="37.9" customHeight="1">
@@ -2051,29 +2051,29 @@
       </c>
       <c r="B45" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская поликлиника №39"</t>
+          <t>СПб ГБУЗ "Городская поликлиника №34"</t>
         </is>
       </c>
       <c r="C45" s="4" t="n">
-        <v>2998</v>
+        <v>417059</v>
       </c>
       <c r="D45" s="4" t="n">
-        <v>8994</v>
+        <v>1615516</v>
       </c>
       <c r="E45" s="4" t="n">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="F45" s="4" t="n">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="G45" s="4" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="H45" s="4" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="I45" s="4" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" ht="37.9" customHeight="1">
@@ -2082,20 +2082,20 @@
       </c>
       <c r="B46" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская поликлиника №51"</t>
+          <t>СПб ГБУЗ "Городская поликлиника №37"</t>
         </is>
       </c>
       <c r="C46" s="4" t="n">
-        <v>23583</v>
+        <v>174</v>
       </c>
       <c r="D46" s="4" t="n">
-        <v>5474</v>
+        <v>1912</v>
       </c>
       <c r="E46" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G46" s="4" t="n">
         <v>0</v>
@@ -2113,26 +2113,26 @@
       </c>
       <c r="B47" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская поликлиника №54"</t>
+          <t>СПб ГБУЗ "Городская поликлиника №38"</t>
         </is>
       </c>
       <c r="C47" s="4" t="n">
-        <v>9945</v>
+        <v>2016</v>
       </c>
       <c r="D47" s="4" t="n">
-        <v>11460</v>
+        <v>2679</v>
       </c>
       <c r="E47" s="4" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F47" s="4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G47" s="4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H47" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I47" s="4" t="n">
         <v>2</v>
@@ -2144,26 +2144,26 @@
       </c>
       <c r="B48" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская поликлиника №63"</t>
+          <t>СПб ГБУЗ "Городская поликлиника №39"</t>
         </is>
       </c>
       <c r="C48" s="4" t="n">
-        <v>4705</v>
+        <v>2998</v>
       </c>
       <c r="D48" s="4" t="n">
-        <v>8500</v>
+        <v>8994</v>
       </c>
       <c r="E48" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="F48" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="F48" s="4" t="n">
-        <v>3</v>
-      </c>
       <c r="G48" s="4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H48" s="4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I48" s="4" t="n">
         <v>0</v>
@@ -2175,20 +2175,20 @@
       </c>
       <c r="B49" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская поликлиника №74"</t>
+          <t>СПб ГБУЗ "Городская поликлиника №51"</t>
         </is>
       </c>
       <c r="C49" s="4" t="n">
-        <v>11996</v>
+        <v>23583</v>
       </c>
       <c r="D49" s="4" t="n">
-        <v>34786</v>
+        <v>5474</v>
       </c>
       <c r="E49" s="4" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F49" s="4" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G49" s="4" t="n">
         <v>0</v>
@@ -2206,29 +2206,29 @@
       </c>
       <c r="B50" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская поликлиника №75"</t>
+          <t>СПб ГБУЗ "Городская поликлиника №54"</t>
         </is>
       </c>
       <c r="C50" s="4" t="n">
-        <v/>
+        <v>9945</v>
       </c>
       <c r="D50" s="4" t="n">
-        <v/>
+        <v>11460</v>
       </c>
       <c r="E50" s="4" t="n">
-        <v/>
+        <v>8</v>
       </c>
       <c r="F50" s="4" t="n">
-        <v/>
+        <v>5</v>
       </c>
       <c r="G50" s="4" t="n">
-        <v/>
+        <v>5</v>
       </c>
       <c r="H50" s="4" t="n">
-        <v/>
+        <v>3</v>
       </c>
       <c r="I50" s="4" t="n">
-        <v/>
+        <v>2</v>
       </c>
     </row>
     <row r="51" ht="37.9" customHeight="1">
@@ -2237,26 +2237,26 @@
       </c>
       <c r="B51" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская поликлиника №77 Невского района"</t>
+          <t>СПб ГБУЗ "Городская поликлиника №63"</t>
         </is>
       </c>
       <c r="C51" s="4" t="n">
-        <v>8194</v>
+        <v>4705</v>
       </c>
       <c r="D51" s="4" t="n">
-        <v>25595</v>
+        <v>8500</v>
       </c>
       <c r="E51" s="4" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F51" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G51" s="4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H51" s="4" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="I51" s="4" t="n">
         <v>0</v>
@@ -2268,29 +2268,29 @@
       </c>
       <c r="B52" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская поликлиника №87"</t>
+          <t>СПб ГБУЗ "Городская поликлиника №74"</t>
         </is>
       </c>
       <c r="C52" s="4" t="n">
-        <v>83210</v>
+        <v>11996</v>
       </c>
       <c r="D52" s="4" t="n">
-        <v>1557674</v>
+        <v>34786</v>
       </c>
       <c r="E52" s="4" t="n">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="F52" s="4" t="n">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="G52" s="4" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="H52" s="4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I52" s="4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" ht="37.9" customHeight="1">
@@ -2299,26 +2299,26 @@
       </c>
       <c r="B53" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская поликлиника №88"</t>
+          <t>СПб ГБУЗ "Городская поликлиника №75"</t>
         </is>
       </c>
       <c r="C53" s="4" t="n">
-        <v>2572</v>
+        <v>36205</v>
       </c>
       <c r="D53" s="4" t="n">
-        <v>2881</v>
+        <v>74759</v>
       </c>
       <c r="E53" s="4" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="F53" s="4" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G53" s="4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H53" s="4" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I53" s="4" t="n">
         <v>0</v>
@@ -2330,29 +2330,29 @@
       </c>
       <c r="B54" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская поликлиника №91"</t>
+          <t>СПб ГБУЗ "Городская поликлиника №77 Невского района"</t>
         </is>
       </c>
       <c r="C54" s="4" t="n">
-        <v>118118</v>
+        <v>8194</v>
       </c>
       <c r="D54" s="4" t="n">
-        <v>150142</v>
+        <v>25595</v>
       </c>
       <c r="E54" s="4" t="n">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="F54" s="4" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="G54" s="4" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="H54" s="4" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="I54" s="4" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" ht="37.9" customHeight="1">
@@ -2361,29 +2361,29 @@
       </c>
       <c r="B55" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городская туберкулезная больница №2"</t>
+          <t>СПб ГБУЗ "Городская поликлиника №87"</t>
         </is>
       </c>
       <c r="C55" s="4" t="n">
-        <v>10643</v>
+        <v>83210</v>
       </c>
       <c r="D55" s="4" t="n">
-        <v>29910</v>
+        <v>1557674</v>
       </c>
       <c r="E55" s="4" t="n">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="F55" s="4" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G55" s="4" t="n">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="H55" s="4" t="n">
         <v>3</v>
       </c>
       <c r="I55" s="4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" ht="37.9" customHeight="1">
@@ -2392,26 +2392,26 @@
       </c>
       <c r="B56" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городской врачебно-физкультурный диспансер"</t>
+          <t>СПб ГБУЗ "Городская поликлиника №88"</t>
         </is>
       </c>
       <c r="C56" s="4" t="n">
-        <v>27075</v>
+        <v>2572</v>
       </c>
       <c r="D56" s="4" t="n">
-        <v>49939</v>
+        <v>2881</v>
       </c>
       <c r="E56" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F56" s="4" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G56" s="4" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H56" s="4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I56" s="4" t="n">
         <v>0</v>
@@ -2423,29 +2423,29 @@
       </c>
       <c r="B57" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городской клинический онкологический диспансер"</t>
+          <t>СПб ГБУЗ "Городская поликлиника №91"</t>
         </is>
       </c>
       <c r="C57" s="4" t="n">
-        <v>9246</v>
+        <v>118118</v>
       </c>
       <c r="D57" s="4" t="n">
-        <v>69746</v>
+        <v>150142</v>
       </c>
       <c r="E57" s="4" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F57" s="4" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G57" s="4" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H57" s="4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I57" s="4" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58" ht="37.9" customHeight="1">
@@ -2454,29 +2454,29 @@
       </c>
       <c r="B58" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городской кожно-венерологический диспансер"</t>
+          <t>СПб ГБУЗ "Городская психиатрическая больница №7 им.акад.И.П.Павлова"</t>
         </is>
       </c>
       <c r="C58" s="4" t="n">
-        <v>26384</v>
+        <v>856</v>
       </c>
       <c r="D58" s="4" t="n">
-        <v>67490</v>
+        <v>2423</v>
       </c>
       <c r="E58" s="4" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F58" s="4" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G58" s="4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H58" s="4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I58" s="4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" ht="37.9" customHeight="1">
@@ -2485,26 +2485,26 @@
       </c>
       <c r="B59" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городской консультативно-диагностический центр №1"</t>
+          <t>СПб ГБУЗ "Городская туберкулезная больница №2"</t>
         </is>
       </c>
       <c r="C59" s="4" t="n">
-        <v>348447</v>
+        <v>10643</v>
       </c>
       <c r="D59" s="4" t="n">
-        <v>1091851</v>
+        <v>29910</v>
       </c>
       <c r="E59" s="4" t="n">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="F59" s="4" t="n">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="G59" s="4" t="n">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="H59" s="4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I59" s="4" t="n">
         <v>0</v>
@@ -2516,26 +2516,26 @@
       </c>
       <c r="B60" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Городской противотуберкулезный диспансер"</t>
+          <t>СПб ГБУЗ "Городской врачебно-физкультурный диспансер"</t>
         </is>
       </c>
       <c r="C60" s="4" t="n">
-        <v>27365</v>
+        <v>27075</v>
       </c>
       <c r="D60" s="4" t="n">
-        <v>73160</v>
+        <v>49939</v>
       </c>
       <c r="E60" s="4" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F60" s="4" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G60" s="4" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H60" s="4" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I60" s="4" t="n">
         <v>0</v>
@@ -2547,29 +2547,29 @@
       </c>
       <c r="B61" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Госпиталь для ветеранов войн"</t>
+          <t>СПб ГБУЗ "Городской гериатрический медико-социальный центр"</t>
         </is>
       </c>
       <c r="C61" s="4" t="n">
-        <v>40995</v>
+        <v>2999</v>
       </c>
       <c r="D61" s="4" t="n">
-        <v>506207</v>
+        <v>20458</v>
       </c>
       <c r="E61" s="4" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="F61" s="4" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G61" s="4" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="H61" s="4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I61" s="4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" ht="37.9" customHeight="1">
@@ -2578,29 +2578,29 @@
       </c>
       <c r="B62" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "ДГБ №2 святой Марии Магдалины"</t>
+          <t>СПб ГБУЗ "Городской клинический онкологический диспансер"</t>
         </is>
       </c>
       <c r="C62" s="4" t="n">
-        <v>47368</v>
+        <v>9246</v>
       </c>
       <c r="D62" s="4" t="n">
-        <v>140614</v>
+        <v>69746</v>
       </c>
       <c r="E62" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="F62" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="F62" s="4" t="n">
-        <v>17</v>
-      </c>
       <c r="G62" s="4" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="H62" s="4" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I62" s="4" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" ht="37.9" customHeight="1">
@@ -2609,29 +2609,29 @@
       </c>
       <c r="B63" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Детская городская больница №17 Святителя Николая Чудотворца"</t>
+          <t>СПб ГБУЗ "Городской кожно-венерологический диспансер"</t>
         </is>
       </c>
       <c r="C63" s="4" t="n">
-        <v>3487</v>
+        <v>26384</v>
       </c>
       <c r="D63" s="4" t="n">
-        <v>23690</v>
+        <v>67490</v>
       </c>
       <c r="E63" s="4" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F63" s="4" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G63" s="4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H63" s="4" t="n">
         <v>6</v>
       </c>
       <c r="I63" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" ht="37.9" customHeight="1">
@@ -2640,29 +2640,29 @@
       </c>
       <c r="B64" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Детская городская больница №22"</t>
+          <t>СПб ГБУЗ "Городской консультативно-диагностический центр №1"</t>
         </is>
       </c>
       <c r="C64" s="4" t="n">
-        <v>26708</v>
+        <v>348447</v>
       </c>
       <c r="D64" s="4" t="n">
-        <v>119246</v>
+        <v>1091851</v>
       </c>
       <c r="E64" s="4" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F64" s="4" t="n">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="G64" s="4" t="n">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H64" s="4" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="I64" s="4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" ht="37.9" customHeight="1">
@@ -2671,26 +2671,26 @@
       </c>
       <c r="B65" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Детская городская клиническая больница №5 имени Нила Федоровича Филатова"</t>
+          <t>СПб ГБУЗ "Городской противотуберкулезный диспансер"</t>
         </is>
       </c>
       <c r="C65" s="4" t="n">
-        <v>18524</v>
+        <v>27365</v>
       </c>
       <c r="D65" s="4" t="n">
-        <v>189475</v>
+        <v>73160</v>
       </c>
       <c r="E65" s="4" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F65" s="4" t="n">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="G65" s="4" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H65" s="4" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I65" s="4" t="n">
         <v>0</v>
@@ -2702,29 +2702,29 @@
       </c>
       <c r="B66" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Детская городская поликлиника №11"</t>
+          <t>СПб ГБУЗ "Госпиталь для ветеранов войн"</t>
         </is>
       </c>
       <c r="C66" s="4" t="n">
-        <v>3746</v>
+        <v>40995</v>
       </c>
       <c r="D66" s="4" t="n">
-        <v>7279</v>
+        <v>506207</v>
       </c>
       <c r="E66" s="4" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="F66" s="4" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="G66" s="4" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="H66" s="4" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I66" s="4" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" ht="37.9" customHeight="1">
@@ -2733,29 +2733,29 @@
       </c>
       <c r="B67" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Детская городская поликлиника №17"</t>
+          <t>СПб ГБУЗ "ДГБ №2 святой Марии Магдалины"</t>
         </is>
       </c>
       <c r="C67" s="4" t="n">
-        <v>3057</v>
+        <v>47368</v>
       </c>
       <c r="D67" s="4" t="n">
-        <v>21768</v>
+        <v>140614</v>
       </c>
       <c r="E67" s="4" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="F67" s="4" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G67" s="4" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H67" s="4" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I67" s="4" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" ht="37.9" customHeight="1">
@@ -2764,29 +2764,29 @@
       </c>
       <c r="B68" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Детская городская поликлиника №44"</t>
+          <t>СПб ГБУЗ "Детская городская больница Святой Ольги"</t>
         </is>
       </c>
       <c r="C68" s="4" t="n">
-        <v>3948</v>
+        <v>6460</v>
       </c>
       <c r="D68" s="4" t="n">
-        <v>7635</v>
+        <v>82040</v>
       </c>
       <c r="E68" s="4" t="n">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="F68" s="4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G68" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H68" s="4" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="I68" s="4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69" ht="37.9" customHeight="1">
@@ -2795,26 +2795,26 @@
       </c>
       <c r="B69" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Детская городская поликлиника №7"</t>
+          <t>СПб ГБУЗ "Детская городская больница №17 Святителя Николая Чудотворца"</t>
         </is>
       </c>
       <c r="C69" s="4" t="n">
-        <v>23922</v>
+        <v>3487</v>
       </c>
       <c r="D69" s="4" t="n">
-        <v>3528</v>
+        <v>23690</v>
       </c>
       <c r="E69" s="4" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="F69" s="4" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G69" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H69" s="4" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I69" s="4" t="n">
         <v>0</v>
@@ -2826,29 +2826,29 @@
       </c>
       <c r="B70" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Детская городская поликлиника №71"</t>
+          <t>СПб ГБУЗ "Детская городская больница №22"</t>
         </is>
       </c>
       <c r="C70" s="4" t="n">
-        <v>267207</v>
+        <v>26708</v>
       </c>
       <c r="D70" s="4" t="n">
-        <v>1214891</v>
+        <v>119246</v>
       </c>
       <c r="E70" s="4" t="n">
         <v>28</v>
       </c>
       <c r="F70" s="4" t="n">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="G70" s="4" t="n">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="H70" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="I70" s="4" t="n">
         <v>2</v>
-      </c>
-      <c r="I70" s="4" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="71" ht="37.9" customHeight="1">
@@ -2857,26 +2857,26 @@
       </c>
       <c r="B71" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Детская инфекционная больница №3"</t>
+          <t>СПб ГБУЗ "Детская городская клиническая больница №5 имени Нила Федоровича Филатова"</t>
         </is>
       </c>
       <c r="C71" s="4" t="n">
-        <v>34820</v>
+        <v>18524</v>
       </c>
       <c r="D71" s="4" t="n">
-        <v>57056</v>
+        <v>189475</v>
       </c>
       <c r="E71" s="4" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F71" s="4" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G71" s="4" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="H71" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I71" s="4" t="n">
         <v>0</v>
@@ -2888,26 +2888,26 @@
       </c>
       <c r="B72" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Детский санаторий - РЦ "Детские Дюны"</t>
+          <t>СПб ГБУЗ "Детская городская поликлиника №11"</t>
         </is>
       </c>
       <c r="C72" s="4" t="n">
-        <v>359</v>
+        <v>3746</v>
       </c>
       <c r="D72" s="4" t="n">
-        <v>1902</v>
+        <v>7279</v>
       </c>
       <c r="E72" s="4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F72" s="4" t="n">
         <v>2</v>
       </c>
       <c r="G72" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H72" s="4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I72" s="4" t="n">
         <v>0</v>
@@ -2919,29 +2919,29 @@
       </c>
       <c r="B73" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Диагностический Центр №7" (глазной) для взрослого и детского населения</t>
+          <t>СПб ГБУЗ "Детская городская поликлиника №17"</t>
         </is>
       </c>
       <c r="C73" s="4" t="n">
-        <v>2325</v>
+        <v>3057</v>
       </c>
       <c r="D73" s="4" t="n">
-        <v>5915</v>
+        <v>21768</v>
       </c>
       <c r="E73" s="4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F73" s="4" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G73" s="4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H73" s="4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I73" s="4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" ht="37.9" customHeight="1">
@@ -2950,26 +2950,26 @@
       </c>
       <c r="B74" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Женская консультация №18"</t>
+          <t>СПб ГБУЗ "Детская городская поликлиника №44"</t>
         </is>
       </c>
       <c r="C74" s="4" t="n">
-        <v>690</v>
+        <v>3948</v>
       </c>
       <c r="D74" s="4" t="n">
-        <v>1224</v>
+        <v>7635</v>
       </c>
       <c r="E74" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="F74" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F74" s="4" t="n">
-        <v>4</v>
-      </c>
       <c r="G74" s="4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H74" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I74" s="4" t="n">
         <v>0</v>
@@ -2981,26 +2981,26 @@
       </c>
       <c r="B75" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Женская консультация №22"</t>
+          <t>СПб ГБУЗ "Детская городская поликлиника №7"</t>
         </is>
       </c>
       <c r="C75" s="4" t="n">
-        <v>1205</v>
+        <v>23922</v>
       </c>
       <c r="D75" s="4" t="n">
-        <v>3233</v>
+        <v>3528</v>
       </c>
       <c r="E75" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F75" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G75" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H75" s="4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I75" s="4" t="n">
         <v>0</v>
@@ -3012,29 +3012,29 @@
       </c>
       <c r="B76" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "КВД №10 - Клиника дерматологии и венерологии"</t>
+          <t>СПб ГБУЗ "Детская городская поликлиника №71"</t>
         </is>
       </c>
       <c r="C76" s="4" t="n">
-        <v>7891</v>
+        <v>267207</v>
       </c>
       <c r="D76" s="4" t="n">
-        <v>70901</v>
+        <v>1214891</v>
       </c>
       <c r="E76" s="4" t="n">
-        <v/>
+        <v>28</v>
       </c>
       <c r="F76" s="4" t="n">
-        <v/>
+        <v>26</v>
       </c>
       <c r="G76" s="4" t="n">
-        <v/>
+        <v>26</v>
       </c>
       <c r="H76" s="4" t="n">
-        <v/>
+        <v>2</v>
       </c>
       <c r="I76" s="4" t="n">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="77" ht="37.9" customHeight="1">
@@ -3043,29 +3043,29 @@
       </c>
       <c r="B77" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "КНпЦСВМП(о)"</t>
+          <t>СПб ГБУЗ "Детская инфекционная больница №3"</t>
         </is>
       </c>
       <c r="C77" s="4" t="n">
-        <v>87404</v>
+        <v>34820</v>
       </c>
       <c r="D77" s="4" t="n">
-        <v>390670</v>
+        <v>57056</v>
       </c>
       <c r="E77" s="4" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F77" s="4" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G77" s="4" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H77" s="4" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I77" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" ht="37.9" customHeight="1">
@@ -3074,23 +3074,23 @@
       </c>
       <c r="B78" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Клиническая больница Святителя Луки"</t>
+          <t>СПб ГБУЗ "Детский санаторий - РЦ "Детские Дюны"</t>
         </is>
       </c>
       <c r="C78" s="4" t="n">
-        <v>18916</v>
+        <v>359</v>
       </c>
       <c r="D78" s="4" t="n">
-        <v>19124</v>
+        <v>1902</v>
       </c>
       <c r="E78" s="4" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F78" s="4" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G78" s="4" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H78" s="4" t="n">
         <v>3</v>
@@ -3105,29 +3105,29 @@
       </c>
       <c r="B79" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Клиническая инфекционная больница им. С.П. Боткина"</t>
+          <t>СПб ГБУЗ "Диагностический Центр №7" (глазной) для взрослого и детского населения</t>
         </is>
       </c>
       <c r="C79" s="4" t="n">
-        <v>414181</v>
+        <v>2325</v>
       </c>
       <c r="D79" s="4" t="n">
-        <v>769603</v>
+        <v>5915</v>
       </c>
       <c r="E79" s="4" t="n">
-        <v>107</v>
+        <v>5</v>
       </c>
       <c r="F79" s="4" t="n">
-        <v>71</v>
+        <v>5</v>
       </c>
       <c r="G79" s="4" t="n">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="H79" s="4" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="I79" s="4" t="n">
-        <v>31</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80" ht="37.9" customHeight="1">
@@ -3136,29 +3136,29 @@
       </c>
       <c r="B80" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Клиническая ревматологическая больница №25"</t>
+          <t>СПб ГБУЗ "Женская консультация №18"</t>
         </is>
       </c>
       <c r="C80" s="4" t="n">
-        <v>21076</v>
+        <v>690</v>
       </c>
       <c r="D80" s="4" t="n">
-        <v>104445</v>
+        <v>1224</v>
       </c>
       <c r="E80" s="4" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="F80" s="4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G80" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H80" s="4" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="I80" s="4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" ht="37.9" customHeight="1">
@@ -3167,29 +3167,29 @@
       </c>
       <c r="B81" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Кожно-венерологический диспансер №9"</t>
+          <t>СПб ГБУЗ "Женская консультация №22"</t>
         </is>
       </c>
       <c r="C81" s="4" t="n">
-        <v>3037</v>
+        <v>1205</v>
       </c>
       <c r="D81" s="4" t="n">
-        <v>11658</v>
+        <v>3233</v>
       </c>
       <c r="E81" s="4" t="n">
         <v>4</v>
       </c>
       <c r="F81" s="4" t="n">
-        <v/>
+        <v>2</v>
       </c>
       <c r="G81" s="4" t="n">
-        <v/>
+        <v>2</v>
       </c>
       <c r="H81" s="4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I81" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" ht="37.9" customHeight="1">
@@ -3198,29 +3198,29 @@
       </c>
       <c r="B82" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Николаевская больница"</t>
+          <t>СПб ГБУЗ "КВД №10 - Клиника дерматологии и венерологии"</t>
         </is>
       </c>
       <c r="C82" s="4" t="n">
-        <v>510689</v>
+        <v>7891</v>
       </c>
       <c r="D82" s="4" t="n">
-        <v>2328822</v>
+        <v>70901</v>
       </c>
       <c r="E82" s="4" t="n">
-        <v>55</v>
+        <v/>
       </c>
       <c r="F82" s="4" t="n">
-        <v>41</v>
+        <v/>
       </c>
       <c r="G82" s="4" t="n">
-        <v>40</v>
+        <v/>
       </c>
       <c r="H82" s="4" t="n">
-        <v>14</v>
+        <v/>
       </c>
       <c r="I82" s="4" t="n">
-        <v>10</v>
+        <v/>
       </c>
     </row>
     <row r="83" ht="37.9" customHeight="1">
@@ -3229,29 +3229,29 @@
       </c>
       <c r="B83" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Противотуберкулезный диспансер №14"</t>
+          <t>СПб ГБУЗ "КДЦ №85"</t>
         </is>
       </c>
       <c r="C83" s="4" t="n">
-        <v>1174</v>
+        <v>61609</v>
       </c>
       <c r="D83" s="4" t="n">
-        <v>3184</v>
+        <v>1388241</v>
       </c>
       <c r="E83" s="4" t="n">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="F83" s="4" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="G83" s="4" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="H83" s="4" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I83" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" ht="37.9" customHeight="1">
@@ -3260,23 +3260,23 @@
       </c>
       <c r="B84" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Противотуберкулезный диспансер №16"</t>
+          <t>СПб ГБУЗ "КНпЦСВМП(о)"</t>
         </is>
       </c>
       <c r="C84" s="4" t="n">
-        <v>1468</v>
+        <v>87404</v>
       </c>
       <c r="D84" s="4" t="n">
-        <v>6516</v>
+        <v>390670</v>
       </c>
       <c r="E84" s="4" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F84" s="4" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G84" s="4" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="H84" s="4" t="n">
         <v>1</v>
@@ -3291,26 +3291,26 @@
       </c>
       <c r="B85" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Противотуберкулезный диспансер №5"</t>
+          <t>СПб ГБУЗ "Клиническая больница Святителя Луки"</t>
         </is>
       </c>
       <c r="C85" s="4" t="n">
-        <v>7012</v>
+        <v>18916</v>
       </c>
       <c r="D85" s="4" t="n">
-        <v>10973</v>
+        <v>19124</v>
       </c>
       <c r="E85" s="4" t="n">
         <v>12</v>
       </c>
       <c r="F85" s="4" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G85" s="4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H85" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I85" s="4" t="n">
         <v>0</v>
@@ -3322,29 +3322,29 @@
       </c>
       <c r="B86" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Психиатрическая больница №1 им.П.П.Кащенко"</t>
+          <t>СПб ГБУЗ "Клиническая инфекционная больница им. С.П. Боткина"</t>
         </is>
       </c>
       <c r="C86" s="4" t="n">
-        <v>5579</v>
+        <v>414181</v>
       </c>
       <c r="D86" s="4" t="n">
-        <v>15898</v>
+        <v>769603</v>
       </c>
       <c r="E86" s="4" t="n">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="F86" s="4" t="n">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="G86" s="4" t="n">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="H86" s="4" t="n">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="I86" s="4" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="87" ht="37.9" customHeight="1">
@@ -3353,29 +3353,29 @@
       </c>
       <c r="B87" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Пушкинский противотуберкулезный диспансер"</t>
+          <t>СПб ГБУЗ "Клиническая ревматологическая больница №25"</t>
         </is>
       </c>
       <c r="C87" s="4" t="n">
-        <v>2311</v>
+        <v>21076</v>
       </c>
       <c r="D87" s="4" t="n">
-        <v>5993</v>
+        <v>104445</v>
       </c>
       <c r="E87" s="4" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F87" s="4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G87" s="4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H87" s="4" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I87" s="4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" ht="37.9" customHeight="1">
@@ -3384,29 +3384,29 @@
       </c>
       <c r="B88" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Родильный дом №1 (специализированный)"</t>
+          <t>СПб ГБУЗ "Кожно-венерологический диспансер №9"</t>
         </is>
       </c>
       <c r="C88" s="4" t="n">
-        <v>7</v>
+        <v>3037</v>
       </c>
       <c r="D88" s="4" t="n">
-        <v>16207</v>
+        <v>11658</v>
       </c>
       <c r="E88" s="4" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F88" s="4" t="n">
-        <v>5</v>
+        <v/>
       </c>
       <c r="G88" s="4" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="H88" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="I88" s="4" t="n">
         <v>1</v>
-      </c>
-      <c r="I88" s="4" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="89" ht="37.9" customHeight="1">
@@ -3415,29 +3415,29 @@
       </c>
       <c r="B89" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Родильный дом №10"</t>
+          <t>СПб ГБУЗ "Николаевская больница"</t>
         </is>
       </c>
       <c r="C89" s="4" t="n">
-        <v>9229</v>
+        <v>510689</v>
       </c>
       <c r="D89" s="4" t="n">
-        <v>91294</v>
+        <v>2328822</v>
       </c>
       <c r="E89" s="4" t="n">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="F89" s="4" t="n">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="G89" s="4" t="n">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="H89" s="4" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="I89" s="4" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="90" ht="37.9" customHeight="1">
@@ -3446,26 +3446,26 @@
       </c>
       <c r="B90" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Родильный дом №13"</t>
+          <t>СПб ГБУЗ "Противотуберкулезный диспансер №14"</t>
         </is>
       </c>
       <c r="C90" s="4" t="n">
-        <v>5192</v>
+        <v>1174</v>
       </c>
       <c r="D90" s="4" t="n">
-        <v>22858</v>
+        <v>3184</v>
       </c>
       <c r="E90" s="4" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F90" s="4" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G90" s="4" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H90" s="4" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I90" s="4" t="n">
         <v>0</v>
@@ -3477,26 +3477,26 @@
       </c>
       <c r="B91" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Родильный дом №16"</t>
+          <t>СПб ГБУЗ "Противотуберкулезный диспансер №16"</t>
         </is>
       </c>
       <c r="C91" s="4" t="n">
-        <v>12177</v>
+        <v>1468</v>
       </c>
       <c r="D91" s="4" t="n">
-        <v>19592</v>
+        <v>6516</v>
       </c>
       <c r="E91" s="4" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F91" s="4" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G91" s="4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H91" s="4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I91" s="4" t="n">
         <v>1</v>
@@ -3508,26 +3508,26 @@
       </c>
       <c r="B92" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Родильный дом №17"</t>
+          <t>СПб ГБУЗ "Противотуберкулезный диспансер №5"</t>
         </is>
       </c>
       <c r="C92" s="4" t="n">
-        <v>6300</v>
+        <v>7012</v>
       </c>
       <c r="D92" s="4" t="n">
-        <v>18610</v>
+        <v>10973</v>
       </c>
       <c r="E92" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="F92" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G92" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H92" s="4" t="n">
         <v>4</v>
-      </c>
-      <c r="F92" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="G92" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H92" s="4" t="n">
-        <v>2</v>
       </c>
       <c r="I92" s="4" t="n">
         <v>0</v>
@@ -3539,26 +3539,26 @@
       </c>
       <c r="B93" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Родильный дом №6 им. проф. В.Ф.Снегирева"</t>
+          <t>СПб ГБУЗ "Психиатрическая больница №1 им.П.П.Кащенко"</t>
         </is>
       </c>
       <c r="C93" s="4" t="n">
-        <v>7246</v>
+        <v>5579</v>
       </c>
       <c r="D93" s="4" t="n">
-        <v>8540</v>
+        <v>15898</v>
       </c>
       <c r="E93" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="F93" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="F93" s="4" t="n">
-        <v>5</v>
-      </c>
       <c r="G93" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H93" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I93" s="4" t="n">
         <v>0</v>
@@ -3570,29 +3570,29 @@
       </c>
       <c r="B94" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Родильный дом №9"</t>
+          <t>СПб ГБУЗ "Пушкинский противотуберкулезный диспансер"</t>
         </is>
       </c>
       <c r="C94" s="4" t="n">
-        <v>8200</v>
+        <v>2311</v>
       </c>
       <c r="D94" s="4" t="n">
-        <v>23200</v>
+        <v>5993</v>
       </c>
       <c r="E94" s="4" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F94" s="4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G94" s="4" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H94" s="4" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I94" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" ht="37.9" customHeight="1">
@@ -3601,29 +3601,29 @@
       </c>
       <c r="B95" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Туберкулезная больница №8"</t>
+          <t>СПб ГБУЗ "Родильный дом №1 (специализированный)"</t>
         </is>
       </c>
       <c r="C95" s="4" t="n">
-        <v>1205</v>
+        <v>7</v>
       </c>
       <c r="D95" s="4" t="n">
-        <v>5660</v>
+        <v>16207</v>
       </c>
       <c r="E95" s="4" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F95" s="4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G95" s="4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H95" s="4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I95" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" ht="37.9" customHeight="1">
@@ -3632,26 +3632,26 @@
       </c>
       <c r="B96" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Центр планирования семьи и репродукции"</t>
+          <t>СПб ГБУЗ "Родильный дом №10"</t>
         </is>
       </c>
       <c r="C96" s="4" t="n">
-        <v>11694</v>
+        <v>9229</v>
       </c>
       <c r="D96" s="4" t="n">
-        <v>14525</v>
+        <v>91294</v>
       </c>
       <c r="E96" s="4" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F96" s="4" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G96" s="4" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H96" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I96" s="4" t="n">
         <v>0</v>
@@ -3663,29 +3663,29 @@
       </c>
       <c r="B97" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ "Центр по профилактике и борьбе со СПИД и инфекционными заболеваниями"</t>
+          <t>СПб ГБУЗ "Родильный дом №13"</t>
         </is>
       </c>
       <c r="C97" s="4" t="n">
-        <v>88446</v>
+        <v>5192</v>
       </c>
       <c r="D97" s="4" t="n">
-        <v>99578</v>
+        <v>22858</v>
       </c>
       <c r="E97" s="4" t="n">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="F97" s="4" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G97" s="4" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="H97" s="4" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="I97" s="4" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" ht="37.9" customHeight="1">
@@ -3694,29 +3694,29 @@
       </c>
       <c r="B98" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ ВЦДОиТ "Огонек"</t>
+          <t>СПб ГБУЗ "Родильный дом №16"</t>
         </is>
       </c>
       <c r="C98" s="4" t="n">
-        <v>154</v>
+        <v>12177</v>
       </c>
       <c r="D98" s="4" t="n">
-        <v>508</v>
+        <v>19592</v>
       </c>
       <c r="E98" s="4" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F98" s="4" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G98" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H98" s="4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I98" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" ht="37.9" customHeight="1">
@@ -3725,29 +3725,29 @@
       </c>
       <c r="B99" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ ГЦОРЗП "Ювента"</t>
+          <t>СПб ГБУЗ "Родильный дом №17"</t>
         </is>
       </c>
       <c r="C99" s="4" t="n">
-        <v>6806</v>
+        <v>6300</v>
       </c>
       <c r="D99" s="4" t="n">
-        <v>9923</v>
+        <v>18610</v>
       </c>
       <c r="E99" s="4" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F99" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G99" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H99" s="4" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I99" s="4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" ht="37.9" customHeight="1">
@@ -3756,26 +3756,26 @@
       </c>
       <c r="B100" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ Детский психоневрологический санаторий "Комарово"</t>
+          <t>СПб ГБУЗ "Родильный дом №6 им. проф. В.Ф.Снегирева"</t>
         </is>
       </c>
       <c r="C100" s="4" t="n">
-        <v>2486</v>
+        <v>7246</v>
       </c>
       <c r="D100" s="4" t="n">
-        <v>212</v>
+        <v>8540</v>
       </c>
       <c r="E100" s="4" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F100" s="4" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G100" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H100" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I100" s="4" t="n">
         <v>0</v>
@@ -3787,29 +3787,29 @@
       </c>
       <c r="B101" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ Детский санаторий "Пионер" (психоневрологический)</t>
+          <t>СПб ГБУЗ "Родильный дом №9"</t>
         </is>
       </c>
       <c r="C101" s="4" t="n">
-        <v>0</v>
+        <v>8200</v>
       </c>
       <c r="D101" s="4" t="n">
-        <v>0</v>
+        <v>23200</v>
       </c>
       <c r="E101" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="F101" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G101" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H101" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="F101" s="4" t="n">
+      <c r="I101" s="4" t="n">
         <v>1</v>
-      </c>
-      <c r="G101" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H101" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I101" s="4" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="102" ht="37.9" customHeight="1">
@@ -3818,29 +3818,29 @@
       </c>
       <c r="B102" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ Детский санаторий "Солнечное"</t>
+          <t>СПб ГБУЗ "Туберкулезная больница №8"</t>
         </is>
       </c>
       <c r="C102" s="4" t="n">
-        <v>355</v>
+        <v>1205</v>
       </c>
       <c r="D102" s="4" t="n">
-        <v>4324</v>
+        <v>5660</v>
       </c>
       <c r="E102" s="4" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F102" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G102" s="4" t="n">
-        <v/>
+        <v>3</v>
       </c>
       <c r="H102" s="4" t="n">
-        <v/>
+        <v>5</v>
       </c>
       <c r="I102" s="4" t="n">
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="103" ht="37.9" customHeight="1">
@@ -3849,29 +3849,29 @@
       </c>
       <c r="B103" s="9" t="inlineStr">
         <is>
-          <t>СПб ГБУЗ КДП № 1</t>
+          <t>СПб ГБУЗ "Центр планирования семьи и репродукции"</t>
         </is>
       </c>
       <c r="C103" s="4" t="n">
-        <v>73234</v>
+        <v>11694</v>
       </c>
       <c r="D103" s="4" t="n">
-        <v>1211453</v>
+        <v>14525</v>
       </c>
       <c r="E103" s="4" t="n">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="F103" s="4" t="n">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="G103" s="4" t="n">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="H103" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I103" s="4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" ht="37.9" customHeight="1">
@@ -3880,29 +3880,29 @@
       </c>
       <c r="B104" s="9" t="inlineStr">
         <is>
-          <t>СПб ГКУЗ "Городская психиатрическая больница №3 им.И.И.Скворцова-Степанова"</t>
+          <t>СПб ГБУЗ "Центр по профилактике и борьбе со СПИД и инфекционными заболеваниями"</t>
         </is>
       </c>
       <c r="C104" s="4" t="n">
-        <v>10439</v>
+        <v>88446</v>
       </c>
       <c r="D104" s="4" t="n">
-        <v>33813</v>
+        <v>99578</v>
       </c>
       <c r="E104" s="4" t="n">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="F104" s="4" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G104" s="4" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H104" s="4" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="I104" s="4" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="105" ht="37.9" customHeight="1">
@@ -3911,26 +3911,26 @@
       </c>
       <c r="B105" s="9" t="inlineStr">
         <is>
-          <t>СПб ГКУЗ "Городская психиатрическая больница №6 (стационар с диспансером)"</t>
+          <t>СПб ГБУЗ ВЦДОиТ "Огонек"</t>
         </is>
       </c>
       <c r="C105" s="4" t="n">
-        <v>3365</v>
+        <v>154</v>
       </c>
       <c r="D105" s="4" t="n">
-        <v>10874</v>
+        <v>508</v>
       </c>
       <c r="E105" s="4" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F105" s="4" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G105" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H105" s="4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I105" s="4" t="n">
         <v>0</v>
@@ -3942,29 +3942,29 @@
       </c>
       <c r="B106" s="9" t="inlineStr">
         <is>
-          <t>СПб ГКУЗ "Диагностический центр (медико-генетический)"</t>
+          <t>СПб ГБУЗ ГЦОРЗП "Ювента"</t>
         </is>
       </c>
       <c r="C106" s="4" t="n">
-        <v>26791</v>
+        <v>6806</v>
       </c>
       <c r="D106" s="4" t="n">
-        <v>36641</v>
+        <v>9923</v>
       </c>
       <c r="E106" s="4" t="n">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F106" s="4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G106" s="4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H106" s="4" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="I106" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107" ht="37.9" customHeight="1">
@@ -3973,29 +3973,29 @@
       </c>
       <c r="B107" s="9" t="inlineStr">
         <is>
-          <t>СПб ГКУЗ "Психиатрическая больница Святого Николая Чудотворца"</t>
+          <t>СПб ГБУЗ Детский психоневрологический санаторий "Комарово"</t>
         </is>
       </c>
       <c r="C107" s="4" t="n">
-        <v>3024</v>
+        <v>2486</v>
       </c>
       <c r="D107" s="4" t="n">
-        <v>20527</v>
+        <v>212</v>
       </c>
       <c r="E107" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F107" s="4" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G107" s="4" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H107" s="4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I107" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" ht="37.9" customHeight="1">
@@ -4004,26 +4004,26 @@
       </c>
       <c r="B108" s="9" t="inlineStr">
         <is>
-          <t>СПб ГКУЗ "Хоспис №1"</t>
+          <t>СПб ГБУЗ Детский санаторий "Пионер" (психоневрологический)</t>
         </is>
       </c>
       <c r="C108" s="4" t="n">
-        <v>297</v>
+        <v>0</v>
       </c>
       <c r="D108" s="4" t="n">
-        <v>3324</v>
+        <v>0</v>
       </c>
       <c r="E108" s="4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F108" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G108" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H108" s="4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I108" s="4" t="n">
         <v>0</v>
@@ -4035,29 +4035,29 @@
       </c>
       <c r="B109" s="9" t="inlineStr">
         <is>
-          <t>СПб ГКУЗ "Хоспис №4"</t>
+          <t>СПб ГБУЗ Детский санаторий "Солнечное"</t>
         </is>
       </c>
       <c r="C109" s="4" t="n">
-        <v>80</v>
+        <v>355</v>
       </c>
       <c r="D109" s="4" t="n">
-        <v>1349</v>
+        <v>4324</v>
       </c>
       <c r="E109" s="4" t="n">
         <v>2</v>
       </c>
       <c r="F109" s="4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G109" s="4" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="H109" s="4" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="I109" s="4" t="n">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="110" ht="37.9" customHeight="1">
@@ -4066,121 +4066,247 @@
       </c>
       <c r="B110" s="9" t="inlineStr">
         <is>
-          <t>СПб ГКУЗ Центр восстановительного лечения "Детская психиатрия" имени С.С. Мнухина</t>
+          <t>СПб ГБУЗ КДП № 1</t>
         </is>
       </c>
       <c r="C110" s="4" t="n">
-        <v>1501</v>
+        <v>73234</v>
       </c>
       <c r="D110" s="4" t="n">
-        <v>5826</v>
+        <v>1211453</v>
       </c>
       <c r="E110" s="4" t="n">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="F110" s="4" t="n">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="G110" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="H110" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="H110" s="4" t="n">
-        <v>0</v>
-      </c>
       <c r="I110" s="4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="111" ht="37.9" customHeight="1">
       <c r="A111" s="4" t="n">
         <v>107</v>
       </c>
-      <c r="B111" s="9" t="n"/>
-      <c r="C111" s="4" t="n"/>
-      <c r="D111" s="4" t="n"/>
-      <c r="E111" s="4" t="n"/>
-      <c r="F111" s="4" t="n"/>
-      <c r="G111" s="4" t="n"/>
-      <c r="H111" s="4" t="n"/>
-      <c r="I111" s="4" t="n"/>
+      <c r="B111" s="9" t="inlineStr">
+        <is>
+          <t>СПб ГКУЗ "Городская психиатрическая больница №3 им.И.И.Скворцова-Степанова"</t>
+        </is>
+      </c>
+      <c r="C111" s="4" t="n">
+        <v>10439</v>
+      </c>
+      <c r="D111" s="4" t="n">
+        <v>33813</v>
+      </c>
+      <c r="E111" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="F111" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="G111" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H111" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="I111" s="4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="112" ht="37.9" customHeight="1">
       <c r="A112" s="4" t="n">
         <v>108</v>
       </c>
-      <c r="B112" s="9" t="n"/>
-      <c r="C112" s="4" t="n"/>
-      <c r="D112" s="4" t="n"/>
-      <c r="E112" s="4" t="n"/>
-      <c r="F112" s="4" t="n"/>
-      <c r="G112" s="4" t="n"/>
-      <c r="H112" s="4" t="n"/>
-      <c r="I112" s="4" t="n"/>
+      <c r="B112" s="9" t="inlineStr">
+        <is>
+          <t>СПб ГКУЗ "Городская психиатрическая больница №6 (стационар с диспансером)"</t>
+        </is>
+      </c>
+      <c r="C112" s="4" t="n">
+        <v>3365</v>
+      </c>
+      <c r="D112" s="4" t="n">
+        <v>10874</v>
+      </c>
+      <c r="E112" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="F112" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G112" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H112" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="I112" s="4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="113" ht="37.9" customHeight="1">
       <c r="A113" s="4" t="n">
         <v>109</v>
       </c>
-      <c r="B113" s="9" t="n"/>
-      <c r="C113" s="4" t="n"/>
-      <c r="D113" s="4" t="n"/>
-      <c r="E113" s="4" t="n"/>
-      <c r="F113" s="4" t="n"/>
-      <c r="G113" s="4" t="n"/>
-      <c r="H113" s="4" t="n"/>
-      <c r="I113" s="4" t="n"/>
+      <c r="B113" s="9" t="inlineStr">
+        <is>
+          <t>СПб ГКУЗ "Диагностический центр (медико-генетический)"</t>
+        </is>
+      </c>
+      <c r="C113" s="4" t="n">
+        <v>26791</v>
+      </c>
+      <c r="D113" s="4" t="n">
+        <v>36641</v>
+      </c>
+      <c r="E113" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="F113" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G113" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H113" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="I113" s="4" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="114" ht="37.9" customHeight="1">
       <c r="A114" s="4" t="n">
         <v>110</v>
       </c>
-      <c r="B114" s="9" t="n"/>
-      <c r="C114" s="4" t="n"/>
-      <c r="D114" s="4" t="n"/>
-      <c r="E114" s="4" t="n"/>
-      <c r="F114" s="4" t="n"/>
-      <c r="G114" s="4" t="n"/>
-      <c r="H114" s="4" t="n"/>
-      <c r="I114" s="4" t="n"/>
+      <c r="B114" s="9" t="inlineStr">
+        <is>
+          <t>СПб ГКУЗ "Психиатрическая больница Святого Николая Чудотворца"</t>
+        </is>
+      </c>
+      <c r="C114" s="4" t="n">
+        <v>3024</v>
+      </c>
+      <c r="D114" s="4" t="n">
+        <v>20527</v>
+      </c>
+      <c r="E114" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="F114" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="G114" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H114" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I114" s="4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="115" ht="37.9" customHeight="1">
       <c r="A115" s="4" t="n">
         <v>111</v>
       </c>
-      <c r="B115" s="9" t="n"/>
-      <c r="C115" s="4" t="n"/>
-      <c r="D115" s="4" t="n"/>
-      <c r="E115" s="4" t="n"/>
-      <c r="F115" s="4" t="n"/>
-      <c r="G115" s="4" t="n"/>
-      <c r="H115" s="4" t="n"/>
-      <c r="I115" s="4" t="n"/>
+      <c r="B115" s="9" t="inlineStr">
+        <is>
+          <t>СПб ГКУЗ "Хоспис №1"</t>
+        </is>
+      </c>
+      <c r="C115" s="4" t="n">
+        <v>297</v>
+      </c>
+      <c r="D115" s="4" t="n">
+        <v>3324</v>
+      </c>
+      <c r="E115" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F115" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G115" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H115" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="I115" s="4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="116" ht="37.9" customHeight="1">
       <c r="A116" s="4" t="n">
         <v>112</v>
       </c>
-      <c r="B116" s="9" t="n"/>
-      <c r="C116" s="4" t="n"/>
-      <c r="D116" s="4" t="n"/>
-      <c r="E116" s="4" t="n"/>
-      <c r="F116" s="4" t="n"/>
-      <c r="G116" s="4" t="n"/>
-      <c r="H116" s="4" t="n"/>
-      <c r="I116" s="4" t="n"/>
+      <c r="B116" s="9" t="inlineStr">
+        <is>
+          <t>СПб ГКУЗ "Хоспис №4"</t>
+        </is>
+      </c>
+      <c r="C116" s="4" t="n">
+        <v>80</v>
+      </c>
+      <c r="D116" s="4" t="n">
+        <v>1349</v>
+      </c>
+      <c r="E116" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F116" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G116" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H116" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I116" s="4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="117" ht="37.9" customHeight="1">
       <c r="A117" s="4" t="n">
         <v>113</v>
       </c>
-      <c r="B117" s="9" t="n"/>
-      <c r="C117" s="4" t="n"/>
-      <c r="D117" s="4" t="n"/>
-      <c r="E117" s="4" t="n"/>
-      <c r="F117" s="4" t="n"/>
-      <c r="G117" s="4" t="n"/>
-      <c r="H117" s="4" t="n"/>
-      <c r="I117" s="4" t="n"/>
+      <c r="B117" s="9" t="inlineStr">
+        <is>
+          <t>СПб ГКУЗ Центр восстановительного лечения "Детская психиатрия" имени С.С. Мнухина</t>
+        </is>
+      </c>
+      <c r="C117" s="4" t="n">
+        <v>1501</v>
+      </c>
+      <c r="D117" s="4" t="n">
+        <v>5826</v>
+      </c>
+      <c r="E117" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="F117" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G117" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="H117" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I117" s="4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="118" ht="37.9" customHeight="1">
       <c r="A118" s="4" t="n">

</xml_diff>